<commit_message>
Changes made by me
</commit_message>
<xml_diff>
--- a/pmo-off.xlsx
+++ b/pmo-off.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -100,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +120,14 @@
       <color rgb="FF333333"/>
       <name val="Georgia"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -142,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -165,11 +173,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF6666FF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF6666FF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -187,6 +206,10 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -483,13 +506,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G45"/>
+  <dimension ref="A2:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="30.75">
       <c r="A2" s="1" t="s">
@@ -1501,6 +1527,14 @@
       </c>
       <c r="G45" s="5">
         <v>139.72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75">
+      <c r="F46" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G46" s="8">
+        <v>19627.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>